<commit_message>
Projeto Traders: Em Desenvolvimento. Projeto Algoritmos: Calculo Nota Corretagem.
</commit_message>
<xml_diff>
--- a/Projeto Traders/Projeto Algoritmos/Algoritmo Calcular Nota Corretagem.xlsx
+++ b/Projeto Traders/Projeto Algoritmos/Algoritmo Calcular Nota Corretagem.xlsx
@@ -210,10 +210,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -266,6 +266,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -273,7 +287,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -283,6 +312,21 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -294,30 +338,41 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -332,30 +387,7 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -370,44 +402,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="45">
     <fill>
@@ -496,175 +496,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -729,17 +729,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -762,26 +756,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -801,6 +777,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -811,155 +802,164 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -968,19 +968,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -998,9 +992,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1027,6 +1018,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1371,7 +1365,7 @@
   <dimension ref="A1:M52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D7" sqref="D7:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1414,7 +1408,7 @@
       <c r="I2">
         <v>1</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="J2" s="14" t="s">
         <v>5</v>
       </c>
       <c r="K2" t="s">
@@ -1441,7 +1435,7 @@
       <c r="I3">
         <v>2</v>
       </c>
-      <c r="J3" s="34"/>
+      <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="5" t="s">
@@ -1453,23 +1447,23 @@
       <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="4">
         <f>D27</f>
-        <v>10.79841</v>
+        <v>10.8</v>
       </c>
       <c r="I4">
         <v>3</v>
       </c>
-      <c r="J4" s="34"/>
+      <c r="J4" s="32"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="8">
         <v>14</v>
       </c>
       <c r="C5" t="s">
@@ -1478,26 +1472,26 @@
       <c r="I5">
         <v>4</v>
       </c>
-      <c r="J5" s="34"/>
+      <c r="J5" s="32"/>
     </row>
     <row r="6" customHeight="1" spans="9:10">
       <c r="I6">
         <v>5</v>
       </c>
-      <c r="J6" s="34"/>
+      <c r="J6" s="32"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="11"/>
+      <c r="E7" s="9"/>
       <c r="I7">
         <v>6</v>
       </c>
-      <c r="J7" s="29"/>
+      <c r="J7" s="27"/>
     </row>
     <row r="8" customHeight="1" spans="1:10">
       <c r="A8" t="s">
@@ -1512,13 +1506,13 @@
       <c r="I8">
         <v>7</v>
       </c>
-      <c r="J8" s="29"/>
+      <c r="J8" s="27"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="11">
         <v>0.09</v>
       </c>
       <c r="C9" t="s">
@@ -1533,13 +1527,13 @@
       <c r="I9">
         <v>8</v>
       </c>
-      <c r="J9" s="29"/>
+      <c r="J9" s="27"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="11">
         <v>9.65</v>
       </c>
       <c r="C10" t="s">
@@ -1554,133 +1548,131 @@
       <c r="I10">
         <v>9</v>
       </c>
-      <c r="J10" s="34"/>
+      <c r="J10" s="32"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="13" t="s">
         <v>25</v>
       </c>
       <c r="I11">
         <v>10</v>
       </c>
-      <c r="J11" s="34"/>
+      <c r="J11" s="32"/>
     </row>
     <row r="12" spans="9:10">
       <c r="I12">
         <v>11</v>
       </c>
-      <c r="J12" s="34"/>
+      <c r="J12" s="32"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16" t="s">
+      <c r="B13" s="14"/>
+      <c r="C13" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D13"/>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17" t="s">
+      <c r="F13" s="9"/>
+      <c r="G13" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="17"/>
+      <c r="H13" s="9"/>
       <c r="I13">
         <v>12</v>
       </c>
-      <c r="J13" s="34"/>
+      <c r="J13" s="32"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="13">
+      <c r="B14" s="15"/>
+      <c r="C14" s="11">
         <f>IF(F15=0,ROUND(((G40*B4)/F33),2),ROUND(((G40*B4)/F33)*F15,2))</f>
         <v>0.3</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="16">
         <f>C14*F14</f>
         <v>0.063</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14" s="11">
         <v>0.21</v>
       </c>
-      <c r="G14" s="20" t="s">
+      <c r="G14" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="11">
         <v>0.21</v>
       </c>
       <c r="I14">
         <v>13</v>
       </c>
-      <c r="J14" s="34"/>
+      <c r="J14" s="32"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="22">
+      <c r="B15" s="18"/>
+      <c r="C15" s="19">
         <f>IF(F15=0,ROUND((((G52)/H45)),2),ROUND((((G52)/F45))*H15,2))</f>
         <v>0.33</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="16">
         <f>C15*H14</f>
         <v>0.0693</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="13">
+      <c r="F15" s="11">
         <v>0.34</v>
       </c>
-      <c r="G15" s="20" t="s">
+      <c r="G15" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="H15" s="13">
+      <c r="H15" s="11">
         <v>0.34</v>
       </c>
       <c r="I15">
         <v>14</v>
       </c>
-      <c r="J15" s="34"/>
+      <c r="J15" s="32"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="23" t="s">
+      <c r="B16" s="18"/>
+      <c r="C16" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D16"/>
       <c r="I16">
         <v>15</v>
       </c>
-      <c r="J16" s="34"/>
+      <c r="J16" s="32"/>
     </row>
     <row r="17" spans="9:10">
       <c r="I17">
         <v>16</v>
       </c>
-      <c r="J17" s="34"/>
+      <c r="J17" s="32"/>
     </row>
     <row r="18" spans="9:10">
       <c r="I18">
         <v>17</v>
       </c>
-      <c r="J18" s="34"/>
+      <c r="J18" s="32"/>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
@@ -1689,18 +1681,18 @@
       <c r="I19">
         <v>18</v>
       </c>
-      <c r="J19" s="34"/>
+      <c r="J19" s="32"/>
     </row>
     <row r="20" spans="6:10">
       <c r="F20" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
       <c r="I20">
         <v>19</v>
       </c>
-      <c r="J20" s="34"/>
+      <c r="J20" s="32"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
@@ -1718,34 +1710,34 @@
       <c r="I21">
         <v>20</v>
       </c>
-      <c r="J21" s="34"/>
+      <c r="J21" s="32"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="26">
+      <c r="B22" s="22"/>
+      <c r="C22" s="23">
         <f>B9*B3</f>
         <v>1.26</v>
       </c>
-      <c r="D22" s="27" t="s">
+      <c r="D22" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="28">
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="25">
         <f>ROUND(D14,2)</f>
         <v>0.06</v>
       </c>
-      <c r="H22" s="28">
+      <c r="H22" s="25">
         <f>G22*B3</f>
         <v>0.84</v>
       </c>
       <c r="I22">
         <v>21</v>
       </c>
-      <c r="J22" s="34" t="s">
+      <c r="J22" s="32" t="s">
         <v>41</v>
       </c>
       <c r="K22">
@@ -1754,55 +1746,55 @@
       </c>
     </row>
     <row r="23" spans="1:13">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="26">
+      <c r="B23" s="22"/>
+      <c r="C23" s="23">
         <f>C22*(B10/100)</f>
         <v>0.12159</v>
       </c>
-      <c r="D23" s="27" t="s">
+      <c r="D23" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="28">
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="25">
         <f>ROUND(D15,2)</f>
         <v>0.07</v>
       </c>
-      <c r="H23" s="28">
+      <c r="H23" s="25">
         <f>G23*B3</f>
         <v>0.98</v>
       </c>
-      <c r="I23" s="35"/>
-      <c r="J23" s="29" t="s">
+      <c r="I23" s="33"/>
+      <c r="J23" s="27" t="s">
         <v>44</v>
       </c>
       <c r="K23">
         <f>SUM(K3:K22)</f>
         <v>14</v>
       </c>
-      <c r="L23" s="36" t="s">
+      <c r="L23" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="M23" s="36"/>
+      <c r="M23" s="34"/>
     </row>
     <row r="24" spans="1:13">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="25"/>
-      <c r="C24" s="26" t="str">
+      <c r="B24" s="22"/>
+      <c r="C24" s="23" t="str">
         <f>B11</f>
         <v>ISENTO</v>
       </c>
-      <c r="D24" s="27" t="s">
+      <c r="D24" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="28">
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="25">
         <f>H22+H23</f>
         <v>1.82</v>
       </c>
@@ -1813,56 +1805,56 @@
         <f>K23/21</f>
         <v>0.666666666666667</v>
       </c>
-      <c r="L24" s="36">
+      <c r="L24" s="34">
         <f>K23</f>
         <v>14</v>
       </c>
-      <c r="M24" s="36"/>
+      <c r="M24" s="34"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="26">
-        <f>C22+C23</f>
-        <v>1.38159</v>
+      <c r="B25" s="22"/>
+      <c r="C25" s="23">
+        <f>ROUND(C22+C23,2)</f>
+        <v>1.38</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="26">
         <f>C22+G24</f>
         <v>3.08</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D27" s="26">
         <f>B5-C25-G24</f>
-        <v>10.79841</v>
+        <v>10.8</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="26">
         <f>B5-B27</f>
         <v>10.92</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="14" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" ht="15.75" spans="1:4">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -1870,12 +1862,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="30" t="s">
+    <row r="32" ht="15.75" spans="1:7">
+      <c r="A32" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="B32" s="30"/>
-      <c r="C32" s="30" t="s">
+      <c r="B32" s="28"/>
+      <c r="C32" s="28" t="s">
         <v>54</v>
       </c>
       <c r="D32" t="s">
@@ -1888,14 +1880,14 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="31" t="s">
+    <row r="33" ht="15.75" spans="1:7">
+      <c r="A33" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="31" t="s">
+      <c r="B33" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="C33" s="31" t="s">
+      <c r="C33" s="29" t="s">
         <v>60</v>
       </c>
       <c r="D33" t="s">
@@ -1912,14 +1904,14 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="32">
+    <row r="34" ht="15.75" spans="1:7">
+      <c r="A34" s="30">
         <v>1</v>
       </c>
-      <c r="B34" s="32">
+      <c r="B34" s="30">
         <v>10</v>
       </c>
-      <c r="C34" s="32">
+      <c r="C34" s="30">
         <v>0.91</v>
       </c>
       <c r="D34">
@@ -1935,14 +1927,14 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="32">
+    <row r="35" ht="15.75" spans="1:7">
+      <c r="A35" s="30">
         <v>11</v>
       </c>
-      <c r="B35" s="32">
+      <c r="B35" s="30">
         <v>50</v>
       </c>
-      <c r="C35" s="32">
+      <c r="C35" s="30">
         <v>0.81</v>
       </c>
       <c r="D35">
@@ -1958,14 +1950,14 @@
         <v>3.24</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="32">
+    <row r="36" ht="15.75" spans="1:7">
+      <c r="A36" s="30">
         <v>51</v>
       </c>
-      <c r="B36" s="32">
+      <c r="B36" s="30">
         <v>100</v>
       </c>
-      <c r="C36" s="32">
+      <c r="C36" s="30">
         <v>0.78</v>
       </c>
       <c r="D36">
@@ -1981,14 +1973,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
-      <c r="A37" s="32">
+    <row r="37" ht="15.75" spans="1:7">
+      <c r="A37" s="30">
         <v>101</v>
       </c>
-      <c r="B37" s="32">
+      <c r="B37" s="30">
         <v>190</v>
       </c>
-      <c r="C37" s="32">
+      <c r="C37" s="30">
         <v>0.73</v>
       </c>
       <c r="D37">
@@ -2004,14 +1996,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="32">
+    <row r="38" ht="15.75" spans="1:7">
+      <c r="A38" s="30">
         <v>191</v>
       </c>
-      <c r="B38" s="32">
+      <c r="B38" s="30">
         <v>2000</v>
       </c>
-      <c r="C38" s="32">
+      <c r="C38" s="30">
         <v>0.68</v>
       </c>
       <c r="D38">
@@ -2027,12 +2019,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="32" t="s">
+    <row r="39" ht="15.75" spans="1:7">
+      <c r="A39" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="B39" s="32"/>
-      <c r="C39" s="32">
+      <c r="B39" s="30"/>
+      <c r="C39" s="30">
         <v>0.64</v>
       </c>
       <c r="D39">
@@ -2049,7 +2041,7 @@
       </c>
     </row>
     <row r="40" spans="6:7">
-      <c r="F40" s="29" t="s">
+      <c r="F40" s="27" t="s">
         <v>44</v>
       </c>
       <c r="G40">
@@ -2058,9 +2050,9 @@
       </c>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="33"/>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="A41" s="31"/>
+    </row>
+    <row r="43" ht="15.75" spans="1:4">
       <c r="A43" t="s">
         <v>62</v>
       </c>
@@ -2068,12 +2060,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
-      <c r="A44" s="30" t="s">
+    <row r="44" ht="15.75" spans="1:7">
+      <c r="A44" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="B44" s="30"/>
-      <c r="C44" s="30" t="s">
+      <c r="B44" s="28"/>
+      <c r="C44" s="28" t="s">
         <v>54</v>
       </c>
       <c r="D44" t="s">
@@ -2086,14 +2078,14 @@
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
-      <c r="A45" s="31" t="s">
+    <row r="45" ht="15.75" spans="1:7">
+      <c r="A45" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B45" s="31" t="s">
+      <c r="B45" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="C45" s="31" t="s">
+      <c r="C45" s="29" t="s">
         <v>60</v>
       </c>
       <c r="D45" t="s">
@@ -2110,14 +2102,14 @@
         <v>60</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
-      <c r="A46" s="32">
+    <row r="46" ht="15.75" spans="1:7">
+      <c r="A46" s="30">
         <v>1</v>
       </c>
-      <c r="B46" s="32">
+      <c r="B46" s="30">
         <v>10</v>
       </c>
-      <c r="C46" s="32">
+      <c r="C46" s="30">
         <v>1</v>
       </c>
       <c r="D46">
@@ -2133,14 +2125,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
-      <c r="A47" s="32">
+    <row r="47" ht="15.75" spans="1:7">
+      <c r="A47" s="30">
         <v>11</v>
       </c>
-      <c r="B47" s="32">
+      <c r="B47" s="30">
         <v>50</v>
       </c>
-      <c r="C47" s="32">
+      <c r="C47" s="30">
         <v>0.9</v>
       </c>
       <c r="D47">
@@ -2156,14 +2148,14 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
-      <c r="A48" s="32">
+    <row r="48" ht="15.75" spans="1:7">
+      <c r="A48" s="30">
         <v>51</v>
       </c>
-      <c r="B48" s="32">
+      <c r="B48" s="30">
         <v>100</v>
       </c>
-      <c r="C48" s="32">
+      <c r="C48" s="30">
         <v>0.85</v>
       </c>
       <c r="D48">
@@ -2179,14 +2171,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
-      <c r="A49" s="32">
+    <row r="49" ht="15.75" spans="1:7">
+      <c r="A49" s="30">
         <v>101</v>
       </c>
-      <c r="B49" s="32">
+      <c r="B49" s="30">
         <v>190</v>
       </c>
-      <c r="C49" s="32">
+      <c r="C49" s="30">
         <v>0.8</v>
       </c>
       <c r="D49">
@@ -2202,14 +2194,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
-      <c r="A50" s="32">
+    <row r="50" ht="15.75" spans="1:7">
+      <c r="A50" s="30">
         <v>191</v>
       </c>
-      <c r="B50" s="32">
+      <c r="B50" s="30">
         <v>2000</v>
       </c>
-      <c r="C50" s="32">
+      <c r="C50" s="30">
         <v>0.75</v>
       </c>
       <c r="D50">
@@ -2225,12 +2217,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
-      <c r="A51" s="32" t="s">
+    <row r="51" ht="15.75" spans="1:7">
+      <c r="A51" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="B51" s="32"/>
-      <c r="C51" s="32">
+      <c r="B51" s="30"/>
+      <c r="C51" s="30">
         <v>0.69</v>
       </c>
       <c r="D51">
@@ -2247,7 +2239,7 @@
       </c>
     </row>
     <row r="52" spans="6:7">
-      <c r="F52" s="29" t="s">
+      <c r="F52" s="27" t="s">
         <v>44</v>
       </c>
       <c r="G52">

</xml_diff>

<commit_message>
Projeto Traders: Em Desenvolvimento. Projeto Algoritmos: Calculo Nota Corretagem. Projeto Algoritmos: Informe DayTrade. Sistema: DataBase.
</commit_message>
<xml_diff>
--- a/Projeto Traders/Projeto Algoritmos/Algoritmo Calcular Nota Corretagem.xlsx
+++ b/Projeto Traders/Projeto Algoritmos/Algoritmo Calcular Nota Corretagem.xlsx
@@ -19,6 +19,9 @@
     <t>Dados a inserir:</t>
   </si>
   <si>
+    <t>Indice Futuro</t>
+  </si>
+  <si>
     <t>Ultimos 21 Pregões</t>
   </si>
   <si>
@@ -164,9 +167,6 @@
   </si>
   <si>
     <t>Custos Totais com a Corretora:</t>
-  </si>
-  <si>
-    <t>Indice Futuro</t>
   </si>
   <si>
     <t>Tabela de Faixas - Emolumentos</t>
@@ -210,10 +210,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -259,42 +259,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -308,6 +273,43 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -315,10 +317,57 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -330,17 +379,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -348,15 +395,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -369,45 +408,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="45">
     <fill>
@@ -496,181 +496,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -715,30 +715,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -749,30 +725,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -794,10 +746,58 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -814,152 +814,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1018,6 +1018,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1365,7 +1368,7 @@
   <dimension ref="A1:M52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:E7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1387,118 +1390,134 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
       <c r="J1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E2" s="4">
         <f>B27</f>
-        <v>3.08</v>
+        <v>5.72</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E3" s="4">
         <f>B28</f>
-        <v>10.92</v>
+        <v>0.279999999999999</v>
       </c>
       <c r="I3">
         <v>2</v>
       </c>
-      <c r="J3" s="32"/>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="J3" s="33"/>
+      <c r="K3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="6">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" s="4">
         <f>D27</f>
-        <v>10.8</v>
+        <v>0.0499999999999998</v>
+      </c>
+      <c r="F4">
+        <v>19</v>
+      </c>
+      <c r="G4">
+        <f>E4+F4</f>
+        <v>19.05</v>
       </c>
       <c r="I4">
         <v>3</v>
       </c>
-      <c r="J4" s="32"/>
+      <c r="J4" s="33"/>
+      <c r="K4">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="8">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I5">
         <v>4</v>
       </c>
-      <c r="J5" s="32"/>
+      <c r="J5" s="33"/>
     </row>
     <row r="6" customHeight="1" spans="9:10">
       <c r="I6">
         <v>5</v>
       </c>
-      <c r="J6" s="32"/>
+      <c r="J6" s="33"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E7" s="9"/>
       <c r="I7">
         <v>6</v>
       </c>
-      <c r="J7" s="27"/>
+      <c r="J7" s="28"/>
     </row>
     <row r="8" customHeight="1" spans="1:10">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E8">
         <v>0.08</v>
@@ -1506,20 +1525,20 @@
       <c r="I8">
         <v>7</v>
       </c>
-      <c r="J8" s="27"/>
+      <c r="J8" s="28"/>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" s="11">
         <v>0.09</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E9">
         <v>0.05</v>
@@ -1527,20 +1546,20 @@
       <c r="I9">
         <v>8</v>
       </c>
-      <c r="J9" s="27"/>
+      <c r="J9" s="28"/>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" s="11">
         <v>9.65</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E10">
         <v>9.65</v>
@@ -1548,68 +1567,68 @@
       <c r="I10">
         <v>9</v>
       </c>
-      <c r="J10" s="32"/>
+      <c r="J10" s="33"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I11">
         <v>10</v>
       </c>
-      <c r="J11" s="32"/>
+      <c r="J11" s="33"/>
     </row>
     <row r="12" spans="9:10">
       <c r="I12">
         <v>11</v>
       </c>
-      <c r="J12" s="32"/>
+      <c r="J12" s="33"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13">
         <v>12</v>
       </c>
-      <c r="J13" s="32"/>
+      <c r="J13" s="33"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="11">
         <f>IF(F15=0,ROUND(((G40*B4)/F33),2),ROUND(((G40*B4)/F33)*F15,2))</f>
-        <v>0.3</v>
+        <v>0.28</v>
       </c>
       <c r="D14" s="16">
         <f>C14*F14</f>
-        <v>0.063</v>
+        <v>0.0588</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F14" s="11">
         <v>0.21</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H14" s="11">
         <v>0.21</v>
@@ -1617,29 +1636,29 @@
       <c r="I14">
         <v>13</v>
       </c>
-      <c r="J14" s="32"/>
+      <c r="J14" s="33"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="19">
         <f>IF(F15=0,ROUND((((G52)/H45)),2),ROUND((((G52)/F45))*H15,2))</f>
-        <v>0.33</v>
+        <v>0.31</v>
       </c>
       <c r="D15" s="16">
         <f>C15*H14</f>
-        <v>0.0693</v>
+        <v>0.0651</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F15" s="11">
         <v>0.34</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H15" s="11">
         <v>0.34</v>
@@ -1647,82 +1666,82 @@
       <c r="I15">
         <v>14</v>
       </c>
-      <c r="J15" s="32"/>
+      <c r="J15" s="33"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B16" s="18"/>
       <c r="C16" s="20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I16">
         <v>15</v>
       </c>
-      <c r="J16" s="32"/>
+      <c r="J16" s="33"/>
     </row>
     <row r="17" spans="9:10">
       <c r="I17">
         <v>16</v>
       </c>
-      <c r="J17" s="32"/>
+      <c r="J17" s="33"/>
     </row>
     <row r="18" spans="9:10">
       <c r="I18">
         <v>17</v>
       </c>
-      <c r="J18" s="32"/>
+      <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I19">
         <v>18</v>
       </c>
-      <c r="J19" s="32"/>
+      <c r="J19" s="33"/>
     </row>
     <row r="20" spans="6:10">
       <c r="F20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G20" s="21"/>
       <c r="H20" s="21"/>
       <c r="I20">
         <v>19</v>
       </c>
-      <c r="J20" s="32"/>
+      <c r="J20" s="33"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D21" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G21" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I21">
         <v>20</v>
       </c>
-      <c r="J21" s="32"/>
+      <c r="J21" s="33"/>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="22" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B22" s="22"/>
       <c r="C22" s="23">
         <f>B9*B3</f>
-        <v>1.26</v>
+        <v>2.34</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E22" s="24"/>
       <c r="F22" s="24"/>
@@ -1732,30 +1751,30 @@
       </c>
       <c r="H22" s="25">
         <f>G22*B3</f>
-        <v>0.84</v>
+        <v>1.56</v>
       </c>
       <c r="I22">
         <v>21</v>
       </c>
-      <c r="J22" s="32" t="s">
-        <v>41</v>
+      <c r="J22" s="33" t="s">
+        <v>42</v>
       </c>
       <c r="K22">
         <f>B3</f>
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B23" s="22"/>
       <c r="C23" s="23">
         <f>C22*(B10/100)</f>
-        <v>0.12159</v>
+        <v>0.22581</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E23" s="24"/>
       <c r="F23" s="24"/>
@@ -1765,24 +1784,24 @@
       </c>
       <c r="H23" s="25">
         <f>G23*B3</f>
-        <v>0.98</v>
-      </c>
-      <c r="I23" s="33"/>
-      <c r="J23" s="27" t="s">
-        <v>44</v>
+        <v>1.82</v>
+      </c>
+      <c r="I23" s="34"/>
+      <c r="J23" s="28" t="s">
+        <v>45</v>
       </c>
       <c r="K23">
         <f>SUM(K3:K22)</f>
-        <v>14</v>
-      </c>
-      <c r="L23" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="M23" s="34"/>
+        <v>42</v>
+      </c>
+      <c r="L23" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="M23" s="35"/>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B24" s="22"/>
       <c r="C24" s="23" t="str">
@@ -1790,68 +1809,72 @@
         <v>ISENTO</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E24" s="24"/>
       <c r="F24" s="24"/>
       <c r="G24" s="25">
         <f>H22+H23</f>
-        <v>1.82</v>
+        <v>3.38</v>
       </c>
       <c r="J24" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K24">
         <f>K23/21</f>
-        <v>0.666666666666667</v>
-      </c>
-      <c r="L24" s="34">
+        <v>2</v>
+      </c>
+      <c r="L24" s="35">
         <f>K23</f>
-        <v>14</v>
-      </c>
-      <c r="M24" s="34"/>
-    </row>
-    <row r="25" spans="1:3">
+        <v>42</v>
+      </c>
+      <c r="M24" s="35"/>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="22" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B25" s="22"/>
       <c r="C25" s="23">
         <f>ROUND(C22+C23,2)</f>
-        <v>1.38</v>
+        <v>2.57</v>
+      </c>
+      <c r="D25" s="26">
+        <f>C25+G24</f>
+        <v>5.95</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="26">
+        <v>5</v>
+      </c>
+      <c r="B27" s="27">
         <f>C22+G24</f>
-        <v>3.08</v>
+        <v>5.72</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" s="26">
+        <v>13</v>
+      </c>
+      <c r="D27" s="27">
         <f>B5-C25-G24</f>
-        <v>10.8</v>
+        <v>0.0499999999999998</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B28" s="26">
+        <v>10</v>
+      </c>
+      <c r="B28" s="27">
         <f>B5-B27</f>
-        <v>10.92</v>
+        <v>0.279999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="27" t="s">
-        <v>15</v>
+      <c r="A30" s="28" t="s">
+        <v>16</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" ht="15.75" spans="1:4">
@@ -1863,11 +1886,11 @@
       </c>
     </row>
     <row r="32" ht="15.75" spans="1:7">
-      <c r="A32" s="28" t="s">
+      <c r="A32" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28" t="s">
+      <c r="B32" s="29"/>
+      <c r="C32" s="29" t="s">
         <v>54</v>
       </c>
       <c r="D32" t="s">
@@ -1881,37 +1904,37 @@
       </c>
     </row>
     <row r="33" ht="15.75" spans="1:7">
-      <c r="A33" s="29" t="s">
+      <c r="A33" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="29" t="s">
+      <c r="B33" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="C33" s="29" t="s">
+      <c r="C33" s="30" t="s">
         <v>60</v>
       </c>
       <c r="D33" t="s">
         <v>60</v>
       </c>
       <c r="E33" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F33">
         <f>L24</f>
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="G33" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="34" ht="15.75" spans="1:7">
-      <c r="A34" s="30">
+      <c r="A34" s="31">
         <v>1</v>
       </c>
-      <c r="B34" s="30">
+      <c r="B34" s="31">
         <v>10</v>
       </c>
-      <c r="C34" s="30">
+      <c r="C34" s="31">
         <v>0.91</v>
       </c>
       <c r="D34">
@@ -1920,7 +1943,7 @@
       </c>
       <c r="E34">
         <f>F33-D34</f>
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="G34">
         <f t="shared" ref="G34:G39" si="0">D34*C34</f>
@@ -1928,18 +1951,18 @@
       </c>
     </row>
     <row r="35" ht="15.75" spans="1:7">
-      <c r="A35" s="30">
+      <c r="A35" s="31">
         <v>11</v>
       </c>
-      <c r="B35" s="30">
+      <c r="B35" s="31">
         <v>50</v>
       </c>
-      <c r="C35" s="30">
+      <c r="C35" s="31">
         <v>0.81</v>
       </c>
       <c r="D35">
         <f>IF(E34&gt;B35,B35-SUM($D$34:D34),E34)</f>
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="E35">
         <f>E34-D35</f>
@@ -1947,17 +1970,17 @@
       </c>
       <c r="G35">
         <f t="shared" si="0"/>
-        <v>3.24</v>
+        <v>25.92</v>
       </c>
     </row>
     <row r="36" ht="15.75" spans="1:7">
-      <c r="A36" s="30">
+      <c r="A36" s="31">
         <v>51</v>
       </c>
-      <c r="B36" s="30">
+      <c r="B36" s="31">
         <v>100</v>
       </c>
-      <c r="C36" s="30">
+      <c r="C36" s="31">
         <v>0.78</v>
       </c>
       <c r="D36">
@@ -1974,13 +1997,13 @@
       </c>
     </row>
     <row r="37" ht="15.75" spans="1:7">
-      <c r="A37" s="30">
+      <c r="A37" s="31">
         <v>101</v>
       </c>
-      <c r="B37" s="30">
+      <c r="B37" s="31">
         <v>190</v>
       </c>
-      <c r="C37" s="30">
+      <c r="C37" s="31">
         <v>0.73</v>
       </c>
       <c r="D37">
@@ -1997,13 +2020,13 @@
       </c>
     </row>
     <row r="38" ht="15.75" spans="1:7">
-      <c r="A38" s="30">
+      <c r="A38" s="31">
         <v>191</v>
       </c>
-      <c r="B38" s="30">
+      <c r="B38" s="31">
         <v>2000</v>
       </c>
-      <c r="C38" s="30">
+      <c r="C38" s="31">
         <v>0.68</v>
       </c>
       <c r="D38">
@@ -2020,11 +2043,11 @@
       </c>
     </row>
     <row r="39" ht="15.75" spans="1:7">
-      <c r="A39" s="30" t="s">
+      <c r="A39" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="B39" s="30"/>
-      <c r="C39" s="30">
+      <c r="B39" s="31"/>
+      <c r="C39" s="31">
         <v>0.64</v>
       </c>
       <c r="D39">
@@ -2041,16 +2064,16 @@
       </c>
     </row>
     <row r="40" spans="6:7">
-      <c r="F40" s="27" t="s">
-        <v>44</v>
+      <c r="F40" s="28" t="s">
+        <v>45</v>
       </c>
       <c r="G40">
         <f>SUM(G34:G39)</f>
-        <v>12.34</v>
+        <v>35.02</v>
       </c>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="31"/>
+      <c r="A41" s="32"/>
     </row>
     <row r="43" ht="15.75" spans="1:4">
       <c r="A43" t="s">
@@ -2061,11 +2084,11 @@
       </c>
     </row>
     <row r="44" ht="15.75" spans="1:7">
-      <c r="A44" s="28" t="s">
+      <c r="A44" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="B44" s="28"/>
-      <c r="C44" s="28" t="s">
+      <c r="B44" s="29"/>
+      <c r="C44" s="29" t="s">
         <v>54</v>
       </c>
       <c r="D44" t="s">
@@ -2079,37 +2102,37 @@
       </c>
     </row>
     <row r="45" ht="15.75" spans="1:7">
-      <c r="A45" s="29" t="s">
+      <c r="A45" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="B45" s="29" t="s">
+      <c r="B45" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="C45" s="29" t="s">
+      <c r="C45" s="30" t="s">
         <v>60</v>
       </c>
       <c r="D45" t="s">
         <v>60</v>
       </c>
       <c r="E45" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F45">
         <f>L24</f>
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="G45" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="46" ht="15.75" spans="1:7">
-      <c r="A46" s="30">
+      <c r="A46" s="31">
         <v>1</v>
       </c>
-      <c r="B46" s="30">
+      <c r="B46" s="31">
         <v>10</v>
       </c>
-      <c r="C46" s="30">
+      <c r="C46" s="31">
         <v>1</v>
       </c>
       <c r="D46">
@@ -2118,7 +2141,7 @@
       </c>
       <c r="E46">
         <f>F45-D46</f>
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="G46">
         <f t="shared" ref="G46:G51" si="1">D46*C46</f>
@@ -2126,18 +2149,18 @@
       </c>
     </row>
     <row r="47" ht="15.75" spans="1:7">
-      <c r="A47" s="30">
+      <c r="A47" s="31">
         <v>11</v>
       </c>
-      <c r="B47" s="30">
+      <c r="B47" s="31">
         <v>50</v>
       </c>
-      <c r="C47" s="30">
+      <c r="C47" s="31">
         <v>0.9</v>
       </c>
       <c r="D47">
         <f>IF(E46&gt;B47,B47-SUM($D$46:D46),E46)</f>
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="E47">
         <f t="shared" ref="E47:E51" si="2">E46-D47</f>
@@ -2145,17 +2168,17 @@
       </c>
       <c r="G47">
         <f t="shared" si="1"/>
-        <v>3.6</v>
+        <v>28.8</v>
       </c>
     </row>
     <row r="48" ht="15.75" spans="1:7">
-      <c r="A48" s="30">
+      <c r="A48" s="31">
         <v>51</v>
       </c>
-      <c r="B48" s="30">
+      <c r="B48" s="31">
         <v>100</v>
       </c>
-      <c r="C48" s="30">
+      <c r="C48" s="31">
         <v>0.85</v>
       </c>
       <c r="D48">
@@ -2172,13 +2195,13 @@
       </c>
     </row>
     <row r="49" ht="15.75" spans="1:7">
-      <c r="A49" s="30">
+      <c r="A49" s="31">
         <v>101</v>
       </c>
-      <c r="B49" s="30">
+      <c r="B49" s="31">
         <v>190</v>
       </c>
-      <c r="C49" s="30">
+      <c r="C49" s="31">
         <v>0.8</v>
       </c>
       <c r="D49">
@@ -2195,13 +2218,13 @@
       </c>
     </row>
     <row r="50" ht="15.75" spans="1:7">
-      <c r="A50" s="30">
+      <c r="A50" s="31">
         <v>191</v>
       </c>
-      <c r="B50" s="30">
+      <c r="B50" s="31">
         <v>2000</v>
       </c>
-      <c r="C50" s="30">
+      <c r="C50" s="31">
         <v>0.75</v>
       </c>
       <c r="D50">
@@ -2218,11 +2241,11 @@
       </c>
     </row>
     <row r="51" ht="15.75" spans="1:7">
-      <c r="A51" s="30" t="s">
+      <c r="A51" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="B51" s="30"/>
-      <c r="C51" s="30">
+      <c r="B51" s="31"/>
+      <c r="C51" s="31">
         <v>0.69</v>
       </c>
       <c r="D51">
@@ -2239,12 +2262,12 @@
       </c>
     </row>
     <row r="52" spans="6:7">
-      <c r="F52" s="27" t="s">
-        <v>44</v>
+      <c r="F52" s="28" t="s">
+        <v>45</v>
       </c>
       <c r="G52">
         <f>SUM(G46:G51)</f>
-        <v>13.6</v>
+        <v>38.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Projeto Traders: Em Desenvolvimento. Projeto Algoritmos: Calculo Nota Corretagem. Sistema: Login.
</commit_message>
<xml_diff>
--- a/Projeto Traders/Projeto Algoritmos/Algoritmo Calcular Nota Corretagem.xlsx
+++ b/Projeto Traders/Projeto Algoritmos/Algoritmo Calcular Nota Corretagem.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78">
   <si>
     <t>Dados a inserir:</t>
   </si>
@@ -25,6 +25,9 @@
     <t>Ultimos 21 Pregões</t>
   </si>
   <si>
+    <t>Calcular</t>
+  </si>
+  <si>
     <t>Ativo:</t>
   </si>
   <si>
@@ -40,6 +43,15 @@
     <t>Contratos Negociados</t>
   </si>
   <si>
+    <t>Lucro/Prejuízo</t>
+  </si>
+  <si>
+    <t>Corretagem Nota</t>
+  </si>
+  <si>
+    <t>Corretagem Unidade</t>
+  </si>
+  <si>
     <t>Contratos:</t>
   </si>
   <si>
@@ -58,24 +70,48 @@
     <t>Total líquido:</t>
   </si>
   <si>
+    <t>13/06/2018</t>
+  </si>
+  <si>
+    <t>Tltal de Contratos:</t>
+  </si>
+  <si>
     <t>Lucro/Prejuizo Bruto:</t>
   </si>
   <si>
     <t>$</t>
   </si>
   <si>
+    <t>14/06/2018</t>
+  </si>
+  <si>
+    <t>Ajuste DayTrade</t>
+  </si>
+  <si>
+    <t>Total das Taxas</t>
+  </si>
+  <si>
+    <t>15/06/2018</t>
+  </si>
+  <si>
     <t>Configuração</t>
   </si>
   <si>
     <t>aproximadamente</t>
   </si>
   <si>
+    <t>ISS/PIS/COFINS:</t>
+  </si>
+  <si>
     <t>Corretora:</t>
   </si>
   <si>
     <t>Registro BMF:</t>
   </si>
   <si>
+    <t>Lucro/Prejuízo:</t>
+  </si>
+  <si>
     <t>Corretagem:</t>
   </si>
   <si>
@@ -155,6 +191,15 @@
   </si>
   <si>
     <t>Numero Inteiro</t>
+  </si>
+  <si>
+    <t>Lucro/Prezjuízo Bruto</t>
+  </si>
+  <si>
+    <t>DARF</t>
+  </si>
+  <si>
+    <t>Liquido</t>
   </si>
   <si>
     <t>Taxa de Intermediação:</t>
@@ -210,12 +255,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,8 +303,127 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -273,47 +437,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -332,82 +460,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="45">
     <fill>
@@ -496,67 +548,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -568,114 +716,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -715,16 +767,75 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -765,201 +876,168 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1039,12 +1117,32 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1365,10 +1463,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:Q52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1383,10 +1481,13 @@
     <col min="9" max="9" width="11.7142857142857"/>
     <col min="10" max="10" width="19.4285714285714" customWidth="1"/>
     <col min="11" max="11" width="22.1428571428571" customWidth="1"/>
-    <col min="12" max="12" width="8.42857142857143" customWidth="1"/>
+    <col min="12" max="12" width="14.8571428571429" customWidth="1"/>
+    <col min="15" max="15" width="17.5714285714286" customWidth="1"/>
+    <col min="16" max="16" width="21.1428571428571" customWidth="1"/>
+    <col min="17" max="17" width="14.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:10">
+    <row r="1" customHeight="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1396,128 +1497,180 @@
       <c r="J1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="O1" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" s="33"/>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E2" s="4">
         <f>B27</f>
-        <v>5.72</v>
+        <v>0</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>8</v>
+      </c>
+      <c r="L2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="P2" s="34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2">
-        <v>26</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B3" s="2"/>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E3" s="4">
         <f>B28</f>
-        <v>0.279999999999999</v>
+        <v>0</v>
       </c>
       <c r="I3">
         <v>2</v>
       </c>
-      <c r="J3" s="33"/>
+      <c r="J3" s="35">
+        <v>43440</v>
+      </c>
       <c r="K3">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>-1.11</v>
+      </c>
+      <c r="O3" s="36"/>
+      <c r="P3" s="34">
+        <f>B9</f>
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" s="5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B4" s="6">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E4" s="4">
         <f>D27</f>
-        <v>0.0499999999999998</v>
-      </c>
-      <c r="F4">
-        <v>19</v>
-      </c>
-      <c r="G4">
-        <f>E4+F4</f>
-        <v>19.05</v>
+        <v>0</v>
       </c>
       <c r="I4">
         <v>3</v>
       </c>
-      <c r="J4" s="33"/>
+      <c r="J4" s="35" t="s">
+        <v>18</v>
+      </c>
       <c r="K4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>14</v>
+      </c>
+      <c r="L4">
+        <v>10.7</v>
+      </c>
+      <c r="O4" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" s="33">
+        <f>O3/P3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="8">
-        <v>6</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B5" s="8"/>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="I5">
         <v>4</v>
       </c>
-      <c r="J5" s="33"/>
-    </row>
-    <row r="6" customHeight="1" spans="9:10">
+      <c r="J5" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>9.46</v>
+      </c>
+      <c r="O5" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="P5" s="34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" customHeight="1" spans="9:16">
       <c r="I6">
         <v>5</v>
       </c>
-      <c r="J6" s="33"/>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="J6" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6">
+        <v>32</v>
+      </c>
+      <c r="L6">
+        <v>-1.31</v>
+      </c>
+      <c r="O6" s="36"/>
+      <c r="P6" s="36"/>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E7" s="9"/>
       <c r="I7">
         <v>6</v>
       </c>
       <c r="J7" s="28"/>
-    </row>
-    <row r="8" customHeight="1" spans="1:10">
+      <c r="O7" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="P7" s="36"/>
+    </row>
+    <row r="8" customHeight="1" spans="1:16">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="E8">
         <v>0.08</v>
@@ -1526,19 +1679,26 @@
         <v>7</v>
       </c>
       <c r="J8" s="28"/>
+      <c r="O8" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="P8" s="33">
+        <f>O6-P6-P7</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="10" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B9" s="11">
         <v>0.09</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="E9">
         <v>0.05</v>
@@ -1550,16 +1710,16 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="10" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B10" s="11">
         <v>9.65</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="E10">
         <v>9.65</v>
@@ -1567,50 +1727,50 @@
       <c r="I10">
         <v>9</v>
       </c>
-      <c r="J10" s="33"/>
+      <c r="J10" s="35"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="12" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="I11">
         <v>10</v>
       </c>
-      <c r="J11" s="33"/>
+      <c r="J11" s="35"/>
     </row>
     <row r="12" spans="9:10">
       <c r="I12">
         <v>11</v>
       </c>
-      <c r="J12" s="33"/>
+      <c r="J12" s="35"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="14" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="14" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="9" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13">
         <v>12</v>
       </c>
-      <c r="J13" s="33"/>
+      <c r="J13" s="35"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="15" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="11">
@@ -1622,13 +1782,13 @@
         <v>0.0588</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="F14" s="11">
         <v>0.21</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="H14" s="11">
         <v>0.21</v>
@@ -1636,11 +1796,11 @@
       <c r="I14">
         <v>13</v>
       </c>
-      <c r="J14" s="33"/>
+      <c r="J14" s="35"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="18" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="19">
@@ -1652,13 +1812,13 @@
         <v>0.0651</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="F15" s="11">
         <v>0.34</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="H15" s="11">
         <v>0.34</v>
@@ -1666,82 +1826,82 @@
       <c r="I15">
         <v>14</v>
       </c>
-      <c r="J15" s="33"/>
+      <c r="J15" s="35"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="18" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="B16" s="18"/>
       <c r="C16" s="20" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="I16">
         <v>15</v>
       </c>
-      <c r="J16" s="33"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="9:10">
       <c r="I17">
         <v>16</v>
       </c>
-      <c r="J17" s="33"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="9:10">
       <c r="I18">
         <v>17</v>
       </c>
-      <c r="J18" s="33"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="I19">
         <v>18</v>
       </c>
-      <c r="J19" s="33"/>
+      <c r="J19" s="35"/>
     </row>
     <row r="20" spans="6:10">
       <c r="F20" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="G20" s="21"/>
       <c r="H20" s="21"/>
       <c r="I20">
         <v>19</v>
       </c>
-      <c r="J20" s="33"/>
+      <c r="J20" s="35"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D21" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="G21" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="H21" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="I21">
         <v>20</v>
       </c>
-      <c r="J21" s="33"/>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="J21" s="35"/>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="22" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="B22" s="22"/>
       <c r="C22" s="23">
         <f>B9*B3</f>
-        <v>2.34</v>
+        <v>0</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="E22" s="24"/>
       <c r="F22" s="24"/>
@@ -1751,30 +1911,34 @@
       </c>
       <c r="H22" s="25">
         <f>G22*B3</f>
-        <v>1.56</v>
+        <v>0</v>
       </c>
       <c r="I22">
         <v>21</v>
       </c>
-      <c r="J22" s="33" t="s">
-        <v>42</v>
+      <c r="J22" s="35" t="s">
+        <v>54</v>
       </c>
       <c r="K22">
         <f>B3</f>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <f>E4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
       <c r="A23" s="22" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B23" s="22"/>
       <c r="C23" s="23">
         <f>C22*(B10/100)</f>
-        <v>0.22581</v>
+        <v>0</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="E23" s="24"/>
       <c r="F23" s="24"/>
@@ -1784,24 +1948,34 @@
       </c>
       <c r="H23" s="25">
         <f>G23*B3</f>
-        <v>1.82</v>
-      </c>
-      <c r="I23" s="34"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="37"/>
       <c r="J23" s="28" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="K23">
         <f>SUM(K3:K22)</f>
-        <v>42</v>
-      </c>
-      <c r="L23" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="M23" s="35"/>
-    </row>
-    <row r="24" spans="1:13">
+        <v>50</v>
+      </c>
+      <c r="L23" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="M23" s="38"/>
+      <c r="N23" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="O23" s="40"/>
+      <c r="P23" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q23" s="41" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
       <c r="A24" s="22" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="B24" s="22"/>
       <c r="C24" s="23" t="str">
@@ -1809,69 +1983,82 @@
         <v>ISENTO</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="E24" s="24"/>
       <c r="F24" s="24"/>
       <c r="G24" s="25">
         <f>H22+H23</f>
-        <v>3.38</v>
+        <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="K24">
         <f>K23/21</f>
-        <v>2</v>
-      </c>
-      <c r="L24" s="35">
+        <v>2.38095238095238</v>
+      </c>
+      <c r="L24" s="38">
         <f>K23</f>
-        <v>42</v>
-      </c>
-      <c r="M24" s="35"/>
+        <v>50</v>
+      </c>
+      <c r="M24" s="38"/>
+      <c r="N24" s="42">
+        <f>SUM(L3:L22)</f>
+        <v>17.74</v>
+      </c>
+      <c r="O24" s="40"/>
+      <c r="P24" s="43">
+        <f>N24*0.2</f>
+        <v>3.548</v>
+      </c>
+      <c r="Q24" s="43">
+        <f>N24-P24</f>
+        <v>14.192</v>
+      </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="22" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="B25" s="22"/>
       <c r="C25" s="23">
         <f>ROUND(C22+C23,2)</f>
-        <v>2.57</v>
+        <v>0</v>
       </c>
       <c r="D25" s="26">
         <f>C25+G24</f>
-        <v>5.95</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B27" s="27">
         <f>C22+G24</f>
-        <v>5.72</v>
+        <v>0</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D27" s="27">
         <f>B5-C25-G24</f>
-        <v>0.0499999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B28" s="27">
         <f>B5-B27</f>
-        <v>0.279999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="28" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B30" s="14" t="s">
         <v>1</v>
@@ -1879,52 +2066,52 @@
     </row>
     <row r="31" ht="15.75" spans="1:4">
       <c r="A31" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="D31" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" ht="15.75" spans="1:7">
       <c r="A32" s="29" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="B32" s="29"/>
       <c r="C32" s="29" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="D32" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="F32" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="G32" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" ht="15.75" spans="1:7">
       <c r="A33" s="30" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="B33" s="30" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="C33" s="30" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D33" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="E33" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="F33">
         <f>L24</f>
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G33" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" ht="15.75" spans="1:7">
@@ -1943,7 +2130,7 @@
       </c>
       <c r="E34">
         <f>F33-D34</f>
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="G34">
         <f t="shared" ref="G34:G39" si="0">D34*C34</f>
@@ -1962,7 +2149,7 @@
       </c>
       <c r="D35">
         <f>IF(E34&gt;B35,B35-SUM($D$34:D34),E34)</f>
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="E35">
         <f>E34-D35</f>
@@ -1970,7 +2157,7 @@
       </c>
       <c r="G35">
         <f t="shared" si="0"/>
-        <v>25.92</v>
+        <v>32.4</v>
       </c>
     </row>
     <row r="36" ht="15.75" spans="1:7">
@@ -2044,7 +2231,7 @@
     </row>
     <row r="39" ht="15.75" spans="1:7">
       <c r="A39" s="31" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="B39" s="31"/>
       <c r="C39" s="31">
@@ -2065,11 +2252,11 @@
     </row>
     <row r="40" spans="6:7">
       <c r="F40" s="28" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="G40">
         <f>SUM(G34:G39)</f>
-        <v>35.02</v>
+        <v>41.5</v>
       </c>
     </row>
     <row r="41" spans="1:1">
@@ -2077,52 +2264,52 @@
     </row>
     <row r="43" ht="15.75" spans="1:4">
       <c r="A43" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="D43" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" ht="15.75" spans="1:7">
       <c r="A44" s="29" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="B44" s="29"/>
       <c r="C44" s="29" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="D44" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="F44" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="G44" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" ht="15.75" spans="1:7">
       <c r="A45" s="30" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="B45" s="30" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="C45" s="30" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D45" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="E45" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="F45">
         <f>L24</f>
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G45" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
     </row>
     <row r="46" ht="15.75" spans="1:7">
@@ -2141,7 +2328,7 @@
       </c>
       <c r="E46">
         <f>F45-D46</f>
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="G46">
         <f t="shared" ref="G46:G51" si="1">D46*C46</f>
@@ -2160,7 +2347,7 @@
       </c>
       <c r="D47">
         <f>IF(E46&gt;B47,B47-SUM($D$46:D46),E46)</f>
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="E47">
         <f t="shared" ref="E47:E51" si="2">E46-D47</f>
@@ -2168,7 +2355,7 @@
       </c>
       <c r="G47">
         <f t="shared" si="1"/>
-        <v>28.8</v>
+        <v>36</v>
       </c>
     </row>
     <row r="48" ht="15.75" spans="1:7">
@@ -2242,7 +2429,7 @@
     </row>
     <row r="51" ht="15.75" spans="1:7">
       <c r="A51" s="31" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="B51" s="31"/>
       <c r="C51" s="31">
@@ -2263,15 +2450,16 @@
     </row>
     <row r="52" spans="6:7">
       <c r="F52" s="28" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="G52">
         <f>SUM(G46:G51)</f>
-        <v>38.8</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="23">
+    <mergeCell ref="O1:P1"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="E13:F13"/>
@@ -2284,9 +2472,11 @@
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="D23:F23"/>
     <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="L24:M24"/>
+    <mergeCell ref="N24:O24"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A39:B39"/>

</xml_diff>

<commit_message>
Projeto Traders: Em Desenvolvimento. Projeto Algoritmos: Calcular Nota. Projeto Conceitual: Projeto Conceitual.
</commit_message>
<xml_diff>
--- a/Projeto Traders/Projeto Algoritmos/Algoritmo Calcular Nota Corretagem.xlsx
+++ b/Projeto Traders/Projeto Algoritmos/Algoritmo Calcular Nota Corretagem.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80">
   <si>
     <t>Dados a inserir:</t>
   </si>
@@ -100,6 +100,9 @@
     <t>aproximadamente</t>
   </si>
   <si>
+    <t>18/06/2018</t>
+  </si>
+  <si>
     <t>ISS/PIS/COFINS:</t>
   </si>
   <si>
@@ -212,6 +215,9 @@
   </si>
   <si>
     <t>Custos Totais com a Corretora:</t>
+  </si>
+  <si>
+    <t>IRRF (1%)</t>
   </si>
   <si>
     <t>Tabela de Faixas - Emolumentos</t>
@@ -255,10 +261,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -311,6 +317,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -318,7 +347,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -332,15 +383,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -354,7 +415,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -368,47 +429,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -423,7 +446,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -437,25 +460,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -548,181 +554,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -792,17 +798,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -810,32 +810,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -858,8 +834,38 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -892,152 +898,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="42" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1120,7 +1126,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1133,12 +1138,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1466,7 +1465,7 @@
   <dimension ref="A1:Q52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1514,7 +1513,7 @@
       </c>
       <c r="E2" s="4">
         <f>B27</f>
-        <v>0</v>
+        <v>9.24</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -1528,10 +1527,10 @@
       <c r="L2" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="34" t="s">
+      <c r="O2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="34" t="s">
+      <c r="P2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1539,7 +1538,9 @@
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2">
+        <v>44</v>
+      </c>
       <c r="C3" t="s">
         <v>13</v>
       </c>
@@ -1548,12 +1549,12 @@
       </c>
       <c r="E3" s="4">
         <f>B28</f>
-        <v>0</v>
+        <v>2.76</v>
       </c>
       <c r="I3">
         <v>2</v>
       </c>
-      <c r="J3" s="35">
+      <c r="J3" s="34">
         <v>43440</v>
       </c>
       <c r="K3">
@@ -1562,8 +1563,8 @@
       <c r="L3">
         <v>-1.11</v>
       </c>
-      <c r="O3" s="36"/>
-      <c r="P3" s="34">
+      <c r="O3" s="35"/>
+      <c r="P3" s="1">
         <f>B9</f>
         <v>0.09</v>
       </c>
@@ -1582,13 +1583,13 @@
         <v>17</v>
       </c>
       <c r="E4" s="4">
-        <f>D27</f>
-        <v>0</v>
+        <f>D27-D28</f>
+        <v>2.36</v>
       </c>
       <c r="I4">
         <v>3</v>
       </c>
-      <c r="J4" s="35" t="s">
+      <c r="J4" s="34" t="s">
         <v>18</v>
       </c>
       <c r="K4">
@@ -1597,7 +1598,7 @@
       <c r="L4">
         <v>10.7</v>
       </c>
-      <c r="O4" s="34" t="s">
+      <c r="O4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="P4" s="33">
@@ -1609,14 +1610,16 @@
       <c r="A5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="8">
+        <v>12</v>
+      </c>
       <c r="C5" t="s">
         <v>21</v>
       </c>
       <c r="I5">
         <v>4</v>
       </c>
-      <c r="J5" s="35" t="s">
+      <c r="J5" s="34" t="s">
         <v>22</v>
       </c>
       <c r="K5">
@@ -1625,10 +1628,10 @@
       <c r="L5">
         <v>9.46</v>
       </c>
-      <c r="O5" s="34" t="s">
+      <c r="O5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="P5" s="34" t="s">
+      <c r="P5" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1636,7 +1639,7 @@
       <c r="I6">
         <v>5</v>
       </c>
-      <c r="J6" s="35" t="s">
+      <c r="J6" s="34" t="s">
         <v>25</v>
       </c>
       <c r="K6">
@@ -1645,8 +1648,8 @@
       <c r="L6">
         <v>-1.31</v>
       </c>
-      <c r="O6" s="36"/>
-      <c r="P6" s="36"/>
+      <c r="O6" s="35"/>
+      <c r="P6" s="35"/>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
@@ -1659,18 +1662,26 @@
       <c r="I7">
         <v>6</v>
       </c>
-      <c r="J7" s="28"/>
-      <c r="O7" s="34" t="s">
+      <c r="J7" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="P7" s="36"/>
+      <c r="K7">
+        <v>14</v>
+      </c>
+      <c r="L7">
+        <v>22.58</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P7" s="35"/>
     </row>
     <row r="8" customHeight="1" spans="1:16">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E8">
         <v>0.08</v>
@@ -1679,8 +1690,8 @@
         <v>7</v>
       </c>
       <c r="J8" s="28"/>
-      <c r="O8" s="34" t="s">
-        <v>31</v>
+      <c r="O8" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="P8" s="33">
         <f>O6-P6-P7</f>
@@ -1689,7 +1700,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B9" s="11">
         <v>0.09</v>
@@ -1698,7 +1709,7 @@
         <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E9">
         <v>0.05</v>
@@ -1710,16 +1721,16 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B10" s="11">
         <v>9.65</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E10">
         <v>9.65</v>
@@ -1727,68 +1738,68 @@
       <c r="I10">
         <v>9</v>
       </c>
-      <c r="J10" s="35"/>
+      <c r="J10" s="34"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I11">
         <v>10</v>
       </c>
-      <c r="J11" s="35"/>
+      <c r="J11" s="34"/>
     </row>
     <row r="12" spans="9:10">
       <c r="I12">
         <v>11</v>
       </c>
-      <c r="J12" s="35"/>
+      <c r="J12" s="34"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="14" t="s">
         <v>21</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13">
         <v>12</v>
       </c>
-      <c r="J13" s="35"/>
+      <c r="J13" s="34"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="11">
         <f>IF(F15=0,ROUND(((G40*B4)/F33),2),ROUND(((G40*B4)/F33)*F15,2))</f>
-        <v>0.28</v>
+        <v>0.27</v>
       </c>
       <c r="D14" s="16">
         <f>C14*F14</f>
-        <v>0.0588</v>
+        <v>0.0567</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F14" s="11">
         <v>0.21</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H14" s="11">
         <v>0.21</v>
@@ -1796,29 +1807,29 @@
       <c r="I14">
         <v>13</v>
       </c>
-      <c r="J14" s="35"/>
+      <c r="J14" s="34"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="18" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="19">
         <f>IF(F15=0,ROUND((((G52)/H45)),2),ROUND((((G52)/F45))*H15,2))</f>
-        <v>0.31</v>
+        <v>0.3</v>
       </c>
       <c r="D15" s="16">
         <f>C15*H14</f>
-        <v>0.0651</v>
+        <v>0.063</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F15" s="11">
         <v>0.34</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H15" s="11">
         <v>0.34</v>
@@ -1826,82 +1837,82 @@
       <c r="I15">
         <v>14</v>
       </c>
-      <c r="J15" s="35"/>
+      <c r="J15" s="34"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B16" s="18"/>
       <c r="C16" s="20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I16">
         <v>15</v>
       </c>
-      <c r="J16" s="35"/>
+      <c r="J16" s="34"/>
     </row>
     <row r="17" spans="9:10">
       <c r="I17">
         <v>16</v>
       </c>
-      <c r="J17" s="35"/>
+      <c r="J17" s="34"/>
     </row>
     <row r="18" spans="9:10">
       <c r="I18">
         <v>17</v>
       </c>
-      <c r="J18" s="35"/>
+      <c r="J18" s="34"/>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I19">
         <v>18</v>
       </c>
-      <c r="J19" s="35"/>
+      <c r="J19" s="34"/>
     </row>
     <row r="20" spans="6:10">
       <c r="F20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G20" s="21"/>
       <c r="H20" s="21"/>
       <c r="I20">
         <v>19</v>
       </c>
-      <c r="J20" s="35"/>
+      <c r="J20" s="34"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G21" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H21" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I21">
         <v>20</v>
       </c>
-      <c r="J21" s="35"/>
+      <c r="J21" s="34"/>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="22" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B22" s="22"/>
       <c r="C22" s="23">
         <f>B9*B3</f>
-        <v>0</v>
+        <v>3.96</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E22" s="24"/>
       <c r="F22" s="24"/>
@@ -1911,71 +1922,71 @@
       </c>
       <c r="H22" s="25">
         <f>G22*B3</f>
-        <v>0</v>
+        <v>2.64</v>
       </c>
       <c r="I22">
         <v>21</v>
       </c>
-      <c r="J22" s="35" t="s">
-        <v>54</v>
+      <c r="J22" s="34" t="s">
+        <v>55</v>
       </c>
       <c r="K22">
         <f>B3</f>
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="L22">
         <f>E4</f>
-        <v>0</v>
+        <v>2.36</v>
       </c>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B23" s="22"/>
       <c r="C23" s="23">
         <f>C22*(B10/100)</f>
-        <v>0</v>
+        <v>0.38214</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E23" s="24"/>
       <c r="F23" s="24"/>
       <c r="G23" s="25">
         <f>ROUND(D15,2)</f>
-        <v>0.07</v>
+        <v>0.06</v>
       </c>
       <c r="H23" s="25">
         <f>G23*B3</f>
-        <v>0</v>
-      </c>
-      <c r="I23" s="37"/>
+        <v>2.64</v>
+      </c>
+      <c r="I23" s="36"/>
       <c r="J23" s="28" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K23">
         <f>SUM(K3:K22)</f>
-        <v>50</v>
-      </c>
-      <c r="L23" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="M23" s="38"/>
-      <c r="N23" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="L23" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="O23" s="40"/>
-      <c r="P23" s="41" t="s">
+      <c r="M23" s="37"/>
+      <c r="N23" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="Q23" s="41" t="s">
+      <c r="O23" s="39"/>
+      <c r="P23" s="40" t="s">
         <v>61</v>
+      </c>
+      <c r="Q23" s="40" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="22" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B24" s="22"/>
       <c r="C24" s="23" t="str">
@@ -1983,52 +1994,52 @@
         <v>ISENTO</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E24" s="24"/>
       <c r="F24" s="24"/>
       <c r="G24" s="25">
         <f>H22+H23</f>
-        <v>0</v>
+        <v>5.28</v>
       </c>
       <c r="J24" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K24">
         <f>K23/21</f>
-        <v>2.38095238095238</v>
-      </c>
-      <c r="L24" s="38">
+        <v>5.14285714285714</v>
+      </c>
+      <c r="L24" s="37">
         <f>K23</f>
-        <v>50</v>
-      </c>
-      <c r="M24" s="38"/>
-      <c r="N24" s="42">
+        <v>108</v>
+      </c>
+      <c r="M24" s="37"/>
+      <c r="N24" s="38">
         <f>SUM(L3:L22)</f>
-        <v>17.74</v>
-      </c>
-      <c r="O24" s="40"/>
-      <c r="P24" s="43">
+        <v>42.68</v>
+      </c>
+      <c r="O24" s="39"/>
+      <c r="P24" s="40">
         <f>N24*0.2</f>
-        <v>3.548</v>
-      </c>
-      <c r="Q24" s="43">
+        <v>8.536</v>
+      </c>
+      <c r="Q24" s="40">
         <f>N24-P24</f>
-        <v>14.192</v>
+        <v>34.144</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B25" s="22"/>
       <c r="C25" s="23">
         <f>ROUND(C22+C23,2)</f>
-        <v>0</v>
+        <v>4.34</v>
       </c>
       <c r="D25" s="26">
         <f>C25+G24</f>
-        <v>0</v>
+        <v>9.62</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2037,23 +2048,30 @@
       </c>
       <c r="B27" s="27">
         <f>C22+G24</f>
-        <v>0</v>
+        <v>9.24</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D27" s="27">
         <f>B5-C25-G24</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
+        <v>2.38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B28" s="27">
         <f>B5-B27</f>
-        <v>0</v>
+        <v>2.76</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" s="14">
+        <f>ROUND(IF(D27&gt;0,D27*0.01,0),2)</f>
+        <v>0.02</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -2066,52 +2084,52 @@
     </row>
     <row r="31" ht="15.75" spans="1:4">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D31" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" ht="15.75" spans="1:7">
       <c r="A32" s="29" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B32" s="29"/>
       <c r="C32" s="29" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D32" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F32" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G32" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" ht="15.75" spans="1:7">
       <c r="A33" s="30" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B33" s="30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C33" s="30" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D33" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E33" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F33">
         <f>L24</f>
-        <v>50</v>
+        <v>108</v>
       </c>
       <c r="G33" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" ht="15.75" spans="1:7">
@@ -2130,7 +2148,7 @@
       </c>
       <c r="E34">
         <f>F33-D34</f>
-        <v>40</v>
+        <v>98</v>
       </c>
       <c r="G34">
         <f t="shared" ref="G34:G39" si="0">D34*C34</f>
@@ -2153,7 +2171,7 @@
       </c>
       <c r="E35">
         <f>E34-D35</f>
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="G35">
         <f t="shared" si="0"/>
@@ -2172,7 +2190,7 @@
       </c>
       <c r="D36">
         <f>IF(E35&gt;B36,B36-SUM($D$34:D35),E35)</f>
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="E36">
         <f>E35-D36</f>
@@ -2180,7 +2198,7 @@
       </c>
       <c r="G36">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>45.24</v>
       </c>
     </row>
     <row r="37" ht="15.75" spans="1:7">
@@ -2231,7 +2249,7 @@
     </row>
     <row r="39" ht="15.75" spans="1:7">
       <c r="A39" s="31" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B39" s="31"/>
       <c r="C39" s="31">
@@ -2252,11 +2270,11 @@
     </row>
     <row r="40" spans="6:7">
       <c r="F40" s="28" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G40">
         <f>SUM(G34:G39)</f>
-        <v>41.5</v>
+        <v>86.74</v>
       </c>
     </row>
     <row r="41" spans="1:1">
@@ -2264,52 +2282,52 @@
     </row>
     <row r="43" ht="15.75" spans="1:4">
       <c r="A43" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D43" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="44" ht="15.75" spans="1:7">
       <c r="A44" s="29" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B44" s="29"/>
       <c r="C44" s="29" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D44" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F44" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G44" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" ht="15.75" spans="1:7">
       <c r="A45" s="30" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B45" s="30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C45" s="30" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D45" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E45" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F45">
         <f>L24</f>
-        <v>50</v>
+        <v>108</v>
       </c>
       <c r="G45" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="46" ht="15.75" spans="1:7">
@@ -2328,7 +2346,7 @@
       </c>
       <c r="E46">
         <f>F45-D46</f>
-        <v>40</v>
+        <v>98</v>
       </c>
       <c r="G46">
         <f t="shared" ref="G46:G51" si="1">D46*C46</f>
@@ -2351,7 +2369,7 @@
       </c>
       <c r="E47">
         <f t="shared" ref="E47:E51" si="2">E46-D47</f>
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="G47">
         <f t="shared" si="1"/>
@@ -2370,7 +2388,7 @@
       </c>
       <c r="D48">
         <f>IF(E47&gt;B48,B48-SUM($D$46:D47),E47)</f>
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="E48">
         <f t="shared" si="2"/>
@@ -2378,7 +2396,7 @@
       </c>
       <c r="G48">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>49.3</v>
       </c>
     </row>
     <row r="49" ht="15.75" spans="1:7">
@@ -2429,7 +2447,7 @@
     </row>
     <row r="51" ht="15.75" spans="1:7">
       <c r="A51" s="31" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B51" s="31"/>
       <c r="C51" s="31">
@@ -2450,11 +2468,11 @@
     </row>
     <row r="52" spans="6:7">
       <c r="F52" s="28" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G52">
         <f>SUM(G46:G51)</f>
-        <v>46</v>
+        <v>95.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Projeto Traders: Em Desenvolvimento. Projeto Algoritmos: Calcular Nota. Projeto Banco de Dados: Projeto Conceitual.
</commit_message>
<xml_diff>
--- a/Projeto Traders/Projeto Algoritmos/Algoritmo Calcular Nota Corretagem.xlsx
+++ b/Projeto Traders/Projeto Algoritmos/Algoritmo Calcular Nota Corretagem.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85">
   <si>
     <t>Dados a inserir:</t>
   </si>
@@ -112,6 +112,9 @@
     <t>Registro BMF:</t>
   </si>
   <si>
+    <t>20/06/2018</t>
+  </si>
+  <si>
     <t>Lucro/Prejuízo:</t>
   </si>
   <si>
@@ -121,6 +124,9 @@
     <t>Emolumentos:</t>
   </si>
   <si>
+    <t>21/06/2018</t>
+  </si>
+  <si>
     <t>Taxa ISS:</t>
   </si>
   <si>
@@ -130,12 +136,18 @@
     <t>ISS, PIS, COFINS:</t>
   </si>
   <si>
+    <t>22/06/2018</t>
+  </si>
+  <si>
     <t>Tx. Intermediação:</t>
   </si>
   <si>
     <t>ISENTO</t>
   </si>
   <si>
+    <t>26/06/2018</t>
+  </si>
+  <si>
     <t>Tarifas da Bolsa de Valores:</t>
   </si>
   <si>
@@ -173,6 +185,9 @@
   </si>
   <si>
     <t>Valor</t>
+  </si>
+  <si>
+    <t>Prejuízo a Compensar</t>
   </si>
   <si>
     <t>Corretagem Total:</t>
@@ -261,9 +276,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
@@ -317,6 +332,103 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -331,61 +443,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <i/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -399,28 +459,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -429,24 +467,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -459,15 +481,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="45">
+  <fills count="46">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -548,43 +563,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -596,139 +749,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -798,11 +819,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -810,8 +837,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -834,38 +876,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -876,6 +888,15 @@
         <color theme="4"/>
       </top>
       <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -898,152 +919,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="42" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="42" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="42" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1130,8 +1151,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1465,7 +1489,7 @@
   <dimension ref="A1:Q52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1513,7 +1537,7 @@
       </c>
       <c r="E2" s="4">
         <f>B27</f>
-        <v>9.24</v>
+        <v>4.4</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -1539,7 +1563,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="2">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -1549,7 +1573,7 @@
       </c>
       <c r="E3" s="4">
         <f>B28</f>
-        <v>2.76</v>
+        <v>-64.4</v>
       </c>
       <c r="I3">
         <v>2</v>
@@ -1563,7 +1587,9 @@
       <c r="L3">
         <v>-1.11</v>
       </c>
-      <c r="O3" s="35"/>
+      <c r="O3" s="35">
+        <v>0.9</v>
+      </c>
       <c r="P3" s="1">
         <f>B9</f>
         <v>0.09</v>
@@ -1584,7 +1610,7 @@
       </c>
       <c r="E4" s="4">
         <f>D27-D28</f>
-        <v>2.36</v>
+        <v>-64.59</v>
       </c>
       <c r="I4">
         <v>3</v>
@@ -1603,7 +1629,7 @@
       </c>
       <c r="P4" s="33">
         <f>O3/P3</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1611,7 +1637,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="8">
-        <v>12</v>
+        <v>-60</v>
       </c>
       <c r="C5" t="s">
         <v>21</v>
@@ -1689,18 +1715,26 @@
       <c r="I8">
         <v>7</v>
       </c>
-      <c r="J8" s="28"/>
+      <c r="J8" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8">
+        <v>46</v>
+      </c>
+      <c r="L8">
+        <v>1.92</v>
+      </c>
       <c r="O8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P8" s="33">
         <f>O6-P6-P7</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:12">
       <c r="A9" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9" s="11">
         <v>0.09</v>
@@ -1709,7 +1743,7 @@
         <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E9">
         <v>0.05</v>
@@ -1717,20 +1751,28 @@
       <c r="I9">
         <v>8</v>
       </c>
-      <c r="J9" s="28"/>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="J9" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="K9">
+        <v>4</v>
+      </c>
+      <c r="L9">
+        <v>8.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="10" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B10" s="11">
         <v>9.65</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E10">
         <v>9.65</v>
@@ -1738,19 +1780,35 @@
       <c r="I10">
         <v>9</v>
       </c>
-      <c r="J10" s="34"/>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="J10" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K10">
+        <v>16</v>
+      </c>
+      <c r="L10">
+        <v>6.29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="12" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I11">
         <v>10</v>
       </c>
-      <c r="J11" s="34"/>
+      <c r="J11" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="K11">
+        <v>10</v>
+      </c>
+      <c r="L11">
+        <v>15.57</v>
+      </c>
     </row>
     <row r="12" spans="9:10">
       <c r="I12">
@@ -1760,18 +1818,18 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="14" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="14" t="s">
         <v>21</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="9" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13">
@@ -1781,25 +1839,25 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="11">
         <f>IF(F15=0,ROUND(((G40*B4)/F33),2),ROUND(((G40*B4)/F33)*F15,2))</f>
-        <v>0.27</v>
+        <v>0.26</v>
       </c>
       <c r="D14" s="16">
         <f>C14*F14</f>
-        <v>0.0567</v>
+        <v>0.0546</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F14" s="11">
         <v>0.21</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="H14" s="11">
         <v>0.21</v>
@@ -1811,25 +1869,25 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="18" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="19">
         <f>IF(F15=0,ROUND((((G52)/H45)),2),ROUND((((G52)/F45))*H15,2))</f>
-        <v>0.3</v>
+        <v>0.29</v>
       </c>
       <c r="D15" s="16">
         <f>C15*H14</f>
-        <v>0.063</v>
+        <v>0.0609</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F15" s="11">
         <v>0.34</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="H15" s="11">
         <v>0.34</v>
@@ -1841,11 +1899,11 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="18" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B16" s="18"/>
       <c r="C16" s="20" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I16">
         <v>15</v>
@@ -1866,7 +1924,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I19">
         <v>18</v>
@@ -1875,7 +1933,7 @@
     </row>
     <row r="20" spans="6:10">
       <c r="F20" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="G20" s="21"/>
       <c r="H20" s="21"/>
@@ -1884,72 +1942,80 @@
       </c>
       <c r="J20" s="34"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:15">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D21" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G21" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="H21" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="I21">
         <v>20</v>
       </c>
       <c r="J21" s="34"/>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="N21" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="O21" s="33"/>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" s="22" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B22" s="22"/>
       <c r="C22" s="23">
         <f>B9*B3</f>
-        <v>3.96</v>
+        <v>1.98</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E22" s="24"/>
       <c r="F22" s="24"/>
       <c r="G22" s="25">
         <f>ROUND(D14,2)</f>
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="H22" s="25">
         <f>G22*B3</f>
-        <v>2.64</v>
+        <v>1.1</v>
       </c>
       <c r="I22">
         <v>21</v>
       </c>
       <c r="J22" s="34" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="K22">
         <f>B3</f>
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="L22">
         <f>E4</f>
-        <v>2.36</v>
-      </c>
+        <v>-64.59</v>
+      </c>
+      <c r="N22" s="36">
+        <v>49.16</v>
+      </c>
+      <c r="O22" s="36"/>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="22" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B23" s="22"/>
       <c r="C23" s="23">
         <f>C22*(B10/100)</f>
-        <v>0.38214</v>
+        <v>0.19107</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E23" s="24"/>
       <c r="F23" s="24"/>
@@ -1959,34 +2025,34 @@
       </c>
       <c r="H23" s="25">
         <f>G23*B3</f>
-        <v>2.64</v>
-      </c>
-      <c r="I23" s="36"/>
+        <v>1.32</v>
+      </c>
+      <c r="I23" s="37"/>
       <c r="J23" s="28" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="K23">
         <f>SUM(K3:K22)</f>
-        <v>108</v>
-      </c>
-      <c r="L23" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="M23" s="37"/>
-      <c r="N23" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="O23" s="39"/>
-      <c r="P23" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q23" s="40" t="s">
-        <v>62</v>
+        <v>162</v>
+      </c>
+      <c r="L23" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="M23" s="38"/>
+      <c r="N23" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="O23" s="40"/>
+      <c r="P23" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q23" s="41" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="22" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B24" s="22"/>
       <c r="C24" s="23" t="str">
@@ -1994,52 +2060,52 @@
         <v>ISENTO</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E24" s="24"/>
       <c r="F24" s="24"/>
       <c r="G24" s="25">
         <f>H22+H23</f>
-        <v>5.28</v>
+        <v>2.42</v>
       </c>
       <c r="J24" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="K24">
         <f>K23/21</f>
-        <v>5.14285714285714</v>
-      </c>
-      <c r="L24" s="37">
+        <v>7.71428571428571</v>
+      </c>
+      <c r="L24" s="38">
         <f>K23</f>
-        <v>108</v>
-      </c>
-      <c r="M24" s="37"/>
-      <c r="N24" s="38">
+        <v>162</v>
+      </c>
+      <c r="M24" s="38"/>
+      <c r="N24" s="39">
         <f>SUM(L3:L22)</f>
-        <v>42.68</v>
-      </c>
-      <c r="O24" s="39"/>
-      <c r="P24" s="40">
-        <f>N24*0.2</f>
-        <v>8.536</v>
-      </c>
-      <c r="Q24" s="40">
-        <f>N24-P24</f>
-        <v>34.144</v>
+        <v>7.52</v>
+      </c>
+      <c r="O24" s="40"/>
+      <c r="P24" s="41">
+        <f>(N24-N22)*0.2</f>
+        <v>-8.328</v>
+      </c>
+      <c r="Q24" s="41">
+        <f>N24-P24-N22</f>
+        <v>-33.312</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="22" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B25" s="22"/>
       <c r="C25" s="23">
         <f>ROUND(C22+C23,2)</f>
-        <v>4.34</v>
+        <v>2.17</v>
       </c>
       <c r="D25" s="26">
         <f>C25+G24</f>
-        <v>9.62</v>
+        <v>4.59</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2048,14 +2114,14 @@
       </c>
       <c r="B27" s="27">
         <f>C22+G24</f>
-        <v>9.24</v>
+        <v>4.4</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D27" s="27">
         <f>B5-C25-G24</f>
-        <v>2.38</v>
+        <v>-64.59</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2064,14 +2130,14 @@
       </c>
       <c r="B28" s="27">
         <f>B5-B27</f>
-        <v>2.76</v>
+        <v>-64.4</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D28" s="14">
         <f>ROUND(IF(D27&gt;0,D27*0.01,0),2)</f>
-        <v>0.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -2084,52 +2150,52 @@
     </row>
     <row r="31" ht="15.75" spans="1:4">
       <c r="A31" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D31" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" ht="15.75" spans="1:7">
       <c r="A32" s="29" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B32" s="29"/>
       <c r="C32" s="29" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D32" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="F32" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="G32" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" ht="15.75" spans="1:7">
       <c r="A33" s="30" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B33" s="30" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C33" s="30" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D33" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E33" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F33">
         <f>L24</f>
-        <v>108</v>
+        <v>162</v>
       </c>
       <c r="G33" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" ht="15.75" spans="1:7">
@@ -2148,7 +2214,7 @@
       </c>
       <c r="E34">
         <f>F33-D34</f>
-        <v>98</v>
+        <v>152</v>
       </c>
       <c r="G34">
         <f t="shared" ref="G34:G39" si="0">D34*C34</f>
@@ -2171,7 +2237,7 @@
       </c>
       <c r="E35">
         <f>E34-D35</f>
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="G35">
         <f t="shared" si="0"/>
@@ -2190,15 +2256,15 @@
       </c>
       <c r="D36">
         <f>IF(E35&gt;B36,B36-SUM($D$34:D35),E35)</f>
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="E36">
         <f>E35-D36</f>
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="G36">
         <f t="shared" si="0"/>
-        <v>45.24</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" ht="15.75" spans="1:7">
@@ -2213,7 +2279,7 @@
       </c>
       <c r="D37">
         <f>IF(E36&gt;B37,B37-SUM($D$34:D36),E36)</f>
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="E37">
         <f>E36-D37</f>
@@ -2221,7 +2287,7 @@
       </c>
       <c r="G37">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>45.26</v>
       </c>
     </row>
     <row r="38" ht="15.75" spans="1:7">
@@ -2249,7 +2315,7 @@
     </row>
     <row r="39" ht="15.75" spans="1:7">
       <c r="A39" s="31" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B39" s="31"/>
       <c r="C39" s="31">
@@ -2270,11 +2336,11 @@
     </row>
     <row r="40" spans="6:7">
       <c r="F40" s="28" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G40">
         <f>SUM(G34:G39)</f>
-        <v>86.74</v>
+        <v>125.76</v>
       </c>
     </row>
     <row r="41" spans="1:1">
@@ -2282,52 +2348,52 @@
     </row>
     <row r="43" ht="15.75" spans="1:4">
       <c r="A43" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D43" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" ht="15.75" spans="1:7">
       <c r="A44" s="29" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B44" s="29"/>
       <c r="C44" s="29" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D44" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="F44" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="G44" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" ht="15.75" spans="1:7">
       <c r="A45" s="30" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B45" s="30" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C45" s="30" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D45" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E45" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F45">
         <f>L24</f>
-        <v>108</v>
+        <v>162</v>
       </c>
       <c r="G45" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="46" ht="15.75" spans="1:7">
@@ -2346,7 +2412,7 @@
       </c>
       <c r="E46">
         <f>F45-D46</f>
-        <v>98</v>
+        <v>152</v>
       </c>
       <c r="G46">
         <f t="shared" ref="G46:G51" si="1">D46*C46</f>
@@ -2369,7 +2435,7 @@
       </c>
       <c r="E47">
         <f t="shared" ref="E47:E51" si="2">E46-D47</f>
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="G47">
         <f t="shared" si="1"/>
@@ -2388,15 +2454,15 @@
       </c>
       <c r="D48">
         <f>IF(E47&gt;B48,B48-SUM($D$46:D47),E47)</f>
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="E48">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="G48">
         <f t="shared" si="1"/>
-        <v>49.3</v>
+        <v>42.5</v>
       </c>
     </row>
     <row r="49" ht="15.75" spans="1:7">
@@ -2411,7 +2477,7 @@
       </c>
       <c r="D49">
         <f>IF(E48&gt;B49,B49-SUM($D$46:D48),E48)</f>
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="E49">
         <f t="shared" si="2"/>
@@ -2419,7 +2485,7 @@
       </c>
       <c r="G49">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>49.6</v>
       </c>
     </row>
     <row r="50" ht="15.75" spans="1:7">
@@ -2447,7 +2513,7 @@
     </row>
     <row r="51" ht="15.75" spans="1:7">
       <c r="A51" s="31" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B51" s="31"/>
       <c r="C51" s="31">
@@ -2468,15 +2534,15 @@
     </row>
     <row r="52" spans="6:7">
       <c r="F52" s="28" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G52">
         <f>SUM(G46:G51)</f>
-        <v>95.3</v>
+        <v>138.1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="25">
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="A13:B13"/>
@@ -2485,8 +2551,10 @@
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
+    <mergeCell ref="N21:O21"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="D22:F22"/>
+    <mergeCell ref="N22:O22"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="D23:F23"/>
     <mergeCell ref="L23:M23"/>

</xml_diff>

<commit_message>
Projeto: Melhora no Algoritmo Projetos Algoritmos: Operações
</commit_message>
<xml_diff>
--- a/Projeto Traders/Projeto Algoritmos/Algoritmo Calcular Nota Corretagem.xlsx
+++ b/Projeto Traders/Projeto Algoritmos/Algoritmo Calcular Nota Corretagem.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8370"/>
+    <workbookView windowWidth="20385" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Indice e Dólar" sheetId="1" r:id="rId1"/>
@@ -252,10 +252,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -328,13 +328,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -344,10 +337,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -359,6 +352,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -368,7 +383,29 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -376,9 +413,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -390,51 +435,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -443,6 +443,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -450,13 +457,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="46">
     <fill>
@@ -551,43 +551,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -599,7 +689,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -611,72 +707,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -684,48 +726,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -795,17 +795,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -834,21 +843,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -858,11 +852,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -895,148 +895,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="41" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="36" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="36" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1464,8 +1464,8 @@
   <sheetPr/>
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1513,7 +1513,7 @@
       </c>
       <c r="E2" s="4">
         <f>B27</f>
-        <v>3.96</v>
+        <v>1.38</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -1539,7 +1539,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="2">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -1549,14 +1549,14 @@
       </c>
       <c r="E3" s="4">
         <f>B28</f>
-        <v>9.04</v>
+        <v>3.62</v>
       </c>
       <c r="I3">
         <v>2</v>
       </c>
       <c r="J3" s="34"/>
       <c r="O3" s="35">
-        <v>1.62</v>
+        <v>0.9</v>
       </c>
       <c r="P3" s="1">
         <f>B9</f>
@@ -1578,7 +1578,7 @@
       </c>
       <c r="E4" s="4">
         <f>D27-D28</f>
-        <v>8.79</v>
+        <v>3.53</v>
       </c>
       <c r="I4">
         <v>3</v>
@@ -1589,7 +1589,7 @@
       </c>
       <c r="P4" s="33">
         <f>O3/P3</f>
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1597,7 +1597,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="8">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
@@ -1748,11 +1748,11 @@
       <c r="B14" s="15"/>
       <c r="C14" s="11">
         <f>IF(F15=0,ROUND(((G40*B4)/F33),2),ROUND(((G40*B4)/F33)*F15,2))</f>
-        <v>0.29</v>
+        <v>0.31</v>
       </c>
       <c r="D14" s="16">
         <f>C14*F14</f>
-        <v>0.0609</v>
+        <v>0.0651</v>
       </c>
       <c r="E14" s="17" t="s">
         <v>39</v>
@@ -1778,11 +1778,11 @@
       <c r="B15" s="18"/>
       <c r="C15" s="19">
         <f>IF(F15=0,ROUND((((G52)/H45)),2),ROUND((((G52)/F45))*H15,2))</f>
-        <v>0.32</v>
+        <v>0.34</v>
       </c>
       <c r="D15" s="16">
         <f>C15*H14</f>
-        <v>0.0672</v>
+        <v>0.0714</v>
       </c>
       <c r="E15" s="17" t="s">
         <v>41</v>
@@ -1875,7 +1875,7 @@
       <c r="B22" s="22"/>
       <c r="C22" s="23">
         <f>B9*B3</f>
-        <v>1.62</v>
+        <v>0.54</v>
       </c>
       <c r="D22" s="24" t="s">
         <v>51</v>
@@ -1884,11 +1884,11 @@
       <c r="F22" s="24"/>
       <c r="G22" s="25">
         <f>ROUND(D14,2)</f>
-        <v>0.06</v>
+        <v>0.07</v>
       </c>
       <c r="H22" s="25">
         <f>G22*B3</f>
-        <v>1.08</v>
+        <v>0.42</v>
       </c>
       <c r="I22">
         <v>21</v>
@@ -1898,11 +1898,11 @@
       </c>
       <c r="K22">
         <f>B3</f>
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="L22">
         <f>E4</f>
-        <v>8.79</v>
+        <v>3.53</v>
       </c>
       <c r="N22" s="36"/>
       <c r="O22" s="36"/>
@@ -1914,7 +1914,7 @@
       <c r="B23" s="22"/>
       <c r="C23" s="23">
         <f>C22*(B10/100)</f>
-        <v>0.15633</v>
+        <v>0.05211</v>
       </c>
       <c r="D23" s="24" t="s">
         <v>54</v>
@@ -1927,7 +1927,7 @@
       </c>
       <c r="H23" s="25">
         <f>G23*B3</f>
-        <v>1.26</v>
+        <v>0.42</v>
       </c>
       <c r="I23" s="37"/>
       <c r="J23" s="28" t="s">
@@ -1935,7 +1935,7 @@
       </c>
       <c r="K23">
         <f>SUM(K3:K22)</f>
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="L23" s="38" t="s">
         <v>56</v>
@@ -1968,32 +1968,32 @@
       <c r="F24" s="24"/>
       <c r="G24" s="25">
         <f>H22+H23</f>
-        <v>2.34</v>
+        <v>0.84</v>
       </c>
       <c r="J24" t="s">
         <v>62</v>
       </c>
       <c r="K24">
         <f>K23/21</f>
-        <v>0.857142857142857</v>
+        <v>0.285714285714286</v>
       </c>
       <c r="L24" s="38">
         <f>K23</f>
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="M24" s="38"/>
       <c r="N24" s="39">
         <f>SUM(L3:L22)</f>
-        <v>8.79</v>
+        <v>3.53</v>
       </c>
       <c r="O24" s="40"/>
       <c r="P24" s="41">
         <f>(N24-N22)*0.2</f>
-        <v>1.758</v>
+        <v>0.706</v>
       </c>
       <c r="Q24" s="41">
         <f>N24-P24-N22</f>
-        <v>7.032</v>
+        <v>2.824</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2003,11 +2003,11 @@
       <c r="B25" s="22"/>
       <c r="C25" s="23">
         <f>ROUND(C22+C23,2)</f>
-        <v>1.78</v>
+        <v>0.59</v>
       </c>
       <c r="D25" s="26">
         <f>C25+G24</f>
-        <v>4.12</v>
+        <v>1.43</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2016,14 +2016,14 @@
       </c>
       <c r="B27" s="27">
         <f>C22+G24</f>
-        <v>3.96</v>
+        <v>1.38</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D27" s="27">
         <f>B5-C25-G24</f>
-        <v>8.88</v>
+        <v>3.57</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2032,14 +2032,14 @@
       </c>
       <c r="B28" s="27">
         <f>B5-B27</f>
-        <v>9.04</v>
+        <v>3.62</v>
       </c>
       <c r="C28" s="28" t="s">
         <v>64</v>
       </c>
       <c r="D28" s="14">
         <f>ROUND(IF(D27&gt;0,D27*0.01,0),2)</f>
-        <v>0.09</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -2094,7 +2094,7 @@
       </c>
       <c r="F33">
         <f>L24</f>
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="G33" t="s">
         <v>74</v>
@@ -2112,15 +2112,15 @@
       </c>
       <c r="D34">
         <f>IF(F33&gt;B34,B34,F33)</f>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E34">
         <f>F33-D34</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G34">
         <f t="shared" ref="G34:G39" si="0">D34*C34</f>
-        <v>9.1</v>
+        <v>5.46</v>
       </c>
     </row>
     <row r="35" ht="15.75" spans="1:7">
@@ -2135,7 +2135,7 @@
       </c>
       <c r="D35">
         <f>IF(E34&gt;B35,B35-SUM($D$34:D34),E34)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E35">
         <f>E34-D35</f>
@@ -2143,7 +2143,7 @@
       </c>
       <c r="G35">
         <f t="shared" si="0"/>
-        <v>6.48</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" ht="15.75" spans="1:7">
@@ -2242,7 +2242,7 @@
       </c>
       <c r="G40">
         <f>SUM(G34:G39)</f>
-        <v>15.58</v>
+        <v>5.46</v>
       </c>
     </row>
     <row r="41" spans="1:1">
@@ -2292,7 +2292,7 @@
       </c>
       <c r="F45">
         <f>L24</f>
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="G45" t="s">
         <v>74</v>
@@ -2310,15 +2310,15 @@
       </c>
       <c r="D46">
         <f>IF(F45&gt;B46,B46,F45)</f>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E46">
         <f>F45-D46</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G46">
         <f t="shared" ref="G46:G51" si="1">D46*C46</f>
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" ht="15.75" spans="1:7">
@@ -2333,7 +2333,7 @@
       </c>
       <c r="D47">
         <f>IF(E46&gt;B47,B47-SUM($D$46:D46),E46)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E47">
         <f t="shared" ref="E47:E51" si="2">E46-D47</f>
@@ -2341,7 +2341,7 @@
       </c>
       <c r="G47">
         <f t="shared" si="1"/>
-        <v>7.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" ht="15.75" spans="1:7">
@@ -2440,7 +2440,7 @@
       </c>
       <c r="G52">
         <f>SUM(G46:G51)</f>
-        <v>17.2</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Projeto: Análise de Requisitos Arquivo: Requisitos Funcionais
</commit_message>
<xml_diff>
--- a/Projeto Traders/Projeto Algoritmos/Algoritmo Calcular Nota Corretagem.xlsx
+++ b/Projeto Traders/Projeto Algoritmos/Algoritmo Calcular Nota Corretagem.xlsx
@@ -254,8 +254,8 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -307,6 +307,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -321,8 +351,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -337,6 +383,21 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -352,68 +413,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -435,6 +436,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -442,21 +457,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="46">
     <fill>
@@ -551,181 +551,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -799,7 +799,18 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -819,11 +830,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -846,23 +863,17 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -881,162 +892,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="41" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1513,7 +1513,7 @@
       </c>
       <c r="E2" s="4">
         <f>B27</f>
-        <v>1.38</v>
+        <v>2.07</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -1539,7 +1539,8 @@
         <v>12</v>
       </c>
       <c r="B3" s="2">
-        <v>6</v>
+        <f>3*3</f>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -1549,7 +1550,7 @@
       </c>
       <c r="E3" s="4">
         <f>B28</f>
-        <v>3.62</v>
+        <v>-2.07</v>
       </c>
       <c r="I3">
         <v>2</v>
@@ -1578,7 +1579,7 @@
       </c>
       <c r="E4" s="4">
         <f>D27-D28</f>
-        <v>3.53</v>
+        <v>-2.15</v>
       </c>
       <c r="I4">
         <v>3</v>
@@ -1596,9 +1597,7 @@
       <c r="A5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="8">
-        <v>5</v>
-      </c>
+      <c r="B5" s="8"/>
       <c r="C5" t="s">
         <v>20</v>
       </c>
@@ -1875,7 +1874,7 @@
       <c r="B22" s="22"/>
       <c r="C22" s="23">
         <f>B9*B3</f>
-        <v>0.54</v>
+        <v>0.81</v>
       </c>
       <c r="D22" s="24" t="s">
         <v>51</v>
@@ -1888,7 +1887,7 @@
       </c>
       <c r="H22" s="25">
         <f>G22*B3</f>
-        <v>0.42</v>
+        <v>0.63</v>
       </c>
       <c r="I22">
         <v>21</v>
@@ -1898,11 +1897,11 @@
       </c>
       <c r="K22">
         <f>B3</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="L22">
         <f>E4</f>
-        <v>3.53</v>
+        <v>-2.15</v>
       </c>
       <c r="N22" s="36"/>
       <c r="O22" s="36"/>
@@ -1914,7 +1913,7 @@
       <c r="B23" s="22"/>
       <c r="C23" s="23">
         <f>C22*(B10/100)</f>
-        <v>0.05211</v>
+        <v>0.078165</v>
       </c>
       <c r="D23" s="24" t="s">
         <v>54</v>
@@ -1927,7 +1926,7 @@
       </c>
       <c r="H23" s="25">
         <f>G23*B3</f>
-        <v>0.42</v>
+        <v>0.63</v>
       </c>
       <c r="I23" s="37"/>
       <c r="J23" s="28" t="s">
@@ -1935,7 +1934,7 @@
       </c>
       <c r="K23">
         <f>SUM(K3:K22)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="L23" s="38" t="s">
         <v>56</v>
@@ -1968,32 +1967,32 @@
       <c r="F24" s="24"/>
       <c r="G24" s="25">
         <f>H22+H23</f>
-        <v>0.84</v>
+        <v>1.26</v>
       </c>
       <c r="J24" t="s">
         <v>62</v>
       </c>
       <c r="K24">
         <f>K23/21</f>
-        <v>0.285714285714286</v>
+        <v>0.428571428571429</v>
       </c>
       <c r="L24" s="38">
         <f>K23</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="M24" s="38"/>
       <c r="N24" s="39">
         <f>SUM(L3:L22)</f>
-        <v>3.53</v>
+        <v>-2.15</v>
       </c>
       <c r="O24" s="40"/>
       <c r="P24" s="41">
         <f>(N24-N22)*0.2</f>
-        <v>0.706</v>
+        <v>-0.43</v>
       </c>
       <c r="Q24" s="41">
         <f>N24-P24-N22</f>
-        <v>2.824</v>
+        <v>-1.72</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2003,11 +2002,11 @@
       <c r="B25" s="22"/>
       <c r="C25" s="23">
         <f>ROUND(C22+C23,2)</f>
-        <v>0.59</v>
+        <v>0.89</v>
       </c>
       <c r="D25" s="26">
         <f>C25+G24</f>
-        <v>1.43</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2016,14 +2015,14 @@
       </c>
       <c r="B27" s="27">
         <f>C22+G24</f>
-        <v>1.38</v>
+        <v>2.07</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D27" s="27">
         <f>B5-C25-G24</f>
-        <v>3.57</v>
+        <v>-2.15</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2032,14 +2031,14 @@
       </c>
       <c r="B28" s="27">
         <f>B5-B27</f>
-        <v>3.62</v>
+        <v>-2.07</v>
       </c>
       <c r="C28" s="28" t="s">
         <v>64</v>
       </c>
       <c r="D28" s="14">
         <f>ROUND(IF(D27&gt;0,D27*0.01,0),2)</f>
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -2094,7 +2093,7 @@
       </c>
       <c r="F33">
         <f>L24</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G33" t="s">
         <v>74</v>
@@ -2112,7 +2111,7 @@
       </c>
       <c r="D34">
         <f>IF(F33&gt;B34,B34,F33)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E34">
         <f>F33-D34</f>
@@ -2120,7 +2119,7 @@
       </c>
       <c r="G34">
         <f t="shared" ref="G34:G39" si="0">D34*C34</f>
-        <v>5.46</v>
+        <v>8.19</v>
       </c>
     </row>
     <row r="35" ht="15.75" spans="1:7">
@@ -2242,7 +2241,7 @@
       </c>
       <c r="G40">
         <f>SUM(G34:G39)</f>
-        <v>5.46</v>
+        <v>8.19</v>
       </c>
     </row>
     <row r="41" spans="1:1">
@@ -2292,7 +2291,7 @@
       </c>
       <c r="F45">
         <f>L24</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G45" t="s">
         <v>74</v>
@@ -2310,7 +2309,7 @@
       </c>
       <c r="D46">
         <f>IF(F45&gt;B46,B46,F45)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E46">
         <f>F45-D46</f>
@@ -2318,7 +2317,7 @@
       </c>
       <c r="G46">
         <f t="shared" ref="G46:G51" si="1">D46*C46</f>
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" ht="15.75" spans="1:7">
@@ -2440,7 +2439,7 @@
       </c>
       <c r="G52">
         <f>SUM(G46:G51)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>